<commit_message>
binary search and sorting
binary search and sorting
</commit_message>
<xml_diff>
--- a/DSA Problems.xlsx
+++ b/DSA Problems.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\Scaler\scaler-oct21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{653AD94C-2735-4C95-B825-25C8625A85A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D0369C-F3D5-4DEE-AD96-BEEE1E62154C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="166">
   <si>
     <t>S.No.</t>
   </si>
@@ -489,6 +489,45 @@
   </si>
   <si>
     <t>Usage of sets and increment of count</t>
+  </si>
+  <si>
+    <t>Sum the difference</t>
+  </si>
+  <si>
+    <t>QuickSort</t>
+  </si>
+  <si>
+    <t>Maximum Unsorted Subarray</t>
+  </si>
+  <si>
+    <t>Maximum and Minimum Magic</t>
+  </si>
+  <si>
+    <t>Binary Search</t>
+  </si>
+  <si>
+    <t>Sorted Array Insertion Position</t>
+  </si>
+  <si>
+    <t>Search For Range (Count Frequency in Sorted Array)</t>
+  </si>
+  <si>
+    <t>Floor Calculate (Greatest element &lt;= K)</t>
+  </si>
+  <si>
+    <t>Ceil Calculate (Smallest element &gt;= K)</t>
+  </si>
+  <si>
+    <t>Find a Peak Element (Local Maxima)</t>
+  </si>
+  <si>
+    <t>Local Minima</t>
+  </si>
+  <si>
+    <t>Single Element (In Sorted Array)</t>
+  </si>
+  <si>
+    <t>Matrix Search</t>
   </si>
 </sst>
 </file>
@@ -2272,7 +2311,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>554691</xdr:colOff>
+          <xdr:colOff>556260</xdr:colOff>
           <xdr:row>48</xdr:row>
           <xdr:rowOff>7620</xdr:rowOff>
         </xdr:to>
@@ -2284,7 +2323,832 @@
                   <a14:compatExt spid="_x0000_s2099"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DABFF2A-7249-4050-89AB-EE747FD2EAE6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000033080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>48</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>548640</xdr:colOff>
+          <xdr:row>49</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2100" name="Object 52" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2100"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000034080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>49</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>91440</xdr:colOff>
+          <xdr:row>50</xdr:row>
+          <xdr:rowOff>7620</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2101" name="Object 53" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2101"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000035080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>50</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>312420</xdr:colOff>
+          <xdr:row>51</xdr:row>
+          <xdr:rowOff>7620</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2102" name="Object 54" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2102"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000036080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>51</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>556260</xdr:colOff>
+          <xdr:row>51</xdr:row>
+          <xdr:rowOff>167640</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2104" name="Object 56" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2104"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000038080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>52</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>533400</xdr:colOff>
+          <xdr:row>53</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2105" name="Object 57" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2105"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000039080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>53</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>548640</xdr:colOff>
+          <xdr:row>54</xdr:row>
+          <xdr:rowOff>22860</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2106" name="Object 58" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2106"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00003A080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>54</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>144780</xdr:colOff>
+          <xdr:row>54</xdr:row>
+          <xdr:rowOff>175260</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2107" name="Object 59" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2107"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00003B080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>55</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>297180</xdr:colOff>
+          <xdr:row>55</xdr:row>
+          <xdr:rowOff>160020</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2108" name="Object 60" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2108"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00003C080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>56</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>624840</xdr:colOff>
+          <xdr:row>57</xdr:row>
+          <xdr:rowOff>7620</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2109" name="Object 61" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2109"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00003D080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>61</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>480060</xdr:colOff>
+          <xdr:row>62</xdr:row>
+          <xdr:rowOff>22860</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2119" name="Object 71" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2119"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000047080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>60</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>487680</xdr:colOff>
+          <xdr:row>60</xdr:row>
+          <xdr:rowOff>175260</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2120" name="Object 72" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2120"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000048080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>59</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>198120</xdr:colOff>
+          <xdr:row>60</xdr:row>
+          <xdr:rowOff>7620</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2121" name="Object 73" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2121"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000049080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>58</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>533400</xdr:colOff>
+          <xdr:row>58</xdr:row>
+          <xdr:rowOff>175260</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2122" name="Object 74" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2122"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00004A080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>57</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>541020</xdr:colOff>
+          <xdr:row>58</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2123" name="Object 75" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2123"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00004B080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+            </a:solidFill>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>67</xdr:row>
+          <xdr:rowOff>1</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>500456</xdr:colOff>
+          <xdr:row>67</xdr:row>
+          <xdr:rowOff>167641</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2128" name="Object 80" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2128"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{770BA239-3425-4E4D-950B-1B18FE19B962}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2335,24 +3199,24 @@
         <xdr:from>
           <xdr:col>4</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>48</xdr:row>
+          <xdr:row>68</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>548640</xdr:colOff>
-          <xdr:row>49</xdr:row>
-          <xdr:rowOff>901</xdr:rowOff>
+          <xdr:col>5</xdr:col>
+          <xdr:colOff>175708</xdr:colOff>
+          <xdr:row>68</xdr:row>
+          <xdr:rowOff>175260</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="2100" name="Object 52" hidden="1">
+            <xdr:cNvPr id="2129" name="Object 81" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2100"/>
+                  <a14:compatExt spid="_x0000_s2129"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{839692E2-85FB-4E58-90BB-1F570407D988}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61838632-7845-47C8-8712-196F6985FE7B}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2403,24 +3267,24 @@
         <xdr:from>
           <xdr:col>4</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>49</xdr:row>
+          <xdr:row>69</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>94914</xdr:colOff>
-          <xdr:row>50</xdr:row>
-          <xdr:rowOff>7620</xdr:rowOff>
+          <xdr:col>4</xdr:col>
+          <xdr:colOff>364864</xdr:colOff>
+          <xdr:row>69</xdr:row>
+          <xdr:rowOff>167640</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="2101" name="Object 53" hidden="1">
+            <xdr:cNvPr id="2130" name="Object 82" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2101"/>
+                  <a14:compatExt spid="_x0000_s2130"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1A2A3A4-B126-4CFE-B918-F7E0C5C9EF3B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C954D24E-1F36-4A86-93C8-B00FA9FFC31B}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2471,24 +3335,24 @@
         <xdr:from>
           <xdr:col>4</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>50</xdr:row>
+          <xdr:row>70</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>312420</xdr:colOff>
-          <xdr:row>51</xdr:row>
-          <xdr:rowOff>6804</xdr:rowOff>
+          <xdr:colOff>388620</xdr:colOff>
+          <xdr:row>70</xdr:row>
+          <xdr:rowOff>182249</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="2102" name="Object 54" hidden="1">
+            <xdr:cNvPr id="2131" name="Object 83" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2102"/>
+                  <a14:compatExt spid="_x0000_s2131"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6557B5B-BECA-4B6E-BCA5-38F0AB1615A6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{446E4352-C7A5-4839-8127-0FE509656EEE}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2539,24 +3403,24 @@
         <xdr:from>
           <xdr:col>4</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>51</xdr:row>
+          <xdr:row>71</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>556260</xdr:colOff>
-          <xdr:row>51</xdr:row>
-          <xdr:rowOff>171157</xdr:rowOff>
+          <xdr:colOff>409015</xdr:colOff>
+          <xdr:row>72</xdr:row>
+          <xdr:rowOff>7620</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="2104" name="Object 56" hidden="1">
+            <xdr:cNvPr id="2132" name="Object 84" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2104"/>
+                  <a14:compatExt spid="_x0000_s2132"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96A47F57-193E-4918-9196-8C236865CD48}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9393BA58-190A-4069-B603-DC0994640646}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2607,24 +3471,24 @@
         <xdr:from>
           <xdr:col>4</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>52</xdr:row>
+          <xdr:row>72</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>533400</xdr:colOff>
-          <xdr:row>52</xdr:row>
-          <xdr:rowOff>180454</xdr:rowOff>
+          <xdr:colOff>449580</xdr:colOff>
+          <xdr:row>73</xdr:row>
+          <xdr:rowOff>11843</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="2105" name="Object 57" hidden="1">
+            <xdr:cNvPr id="2133" name="Object 85" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2105"/>
+                  <a14:compatExt spid="_x0000_s2133"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72239AC9-600C-4305-A470-639596525BC8}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{424D097F-B5F4-4916-9D1C-37F9A0AEF70D}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2675,24 +3539,24 @@
         <xdr:from>
           <xdr:col>4</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>53</xdr:row>
+          <xdr:row>73</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>548640</xdr:colOff>
-          <xdr:row>54</xdr:row>
-          <xdr:rowOff>20986</xdr:rowOff>
+          <xdr:colOff>406213</xdr:colOff>
+          <xdr:row>74</xdr:row>
+          <xdr:rowOff>7620</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="2106" name="Object 58" hidden="1">
+            <xdr:cNvPr id="2134" name="Object 86" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2106"/>
+                  <a14:compatExt spid="_x0000_s2134"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99367707-ADD5-486A-BC35-B9368808DFFD}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C64A143F-E631-4E18-BB33-988B35289E0E}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2743,500 +3607,24 @@
         <xdr:from>
           <xdr:col>4</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>54</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>147357</xdr:colOff>
-          <xdr:row>54</xdr:row>
-          <xdr:rowOff>175260</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2107" name="Object 59" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2107"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5B99C0C-8815-4907-B8C9-311477600E73}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd type="none" w="med" len="med"/>
-            </a:ln>
-            <a:effectLst/>
-            <a:extLst>
-              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                <a14:hiddenEffects>
-                  <a:effectLst>
-                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                      <a:srgbClr val="808080"/>
-                    </a:outerShdw>
-                  </a:effectLst>
-                </a14:hiddenEffects>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
-          <xdr:row>55</xdr:row>
+          <xdr:row>74</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>297180</xdr:colOff>
-          <xdr:row>55</xdr:row>
-          <xdr:rowOff>160383</xdr:rowOff>
+          <xdr:colOff>701040</xdr:colOff>
+          <xdr:row>75</xdr:row>
+          <xdr:rowOff>3334</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="2108" name="Object 60" hidden="1">
+            <xdr:cNvPr id="2135" name="Object 87" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2108"/>
+                  <a14:compatExt spid="_x0000_s2135"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7EAB8BC6-B1B3-4C2D-ABFB-21AD824589D3}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd type="none" w="med" len="med"/>
-            </a:ln>
-            <a:effectLst/>
-            <a:extLst>
-              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                <a14:hiddenEffects>
-                  <a:effectLst>
-                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                      <a:srgbClr val="808080"/>
-                    </a:outerShdw>
-                  </a:effectLst>
-                </a14:hiddenEffects>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
-          <xdr:row>56</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>624840</xdr:colOff>
-          <xdr:row>57</xdr:row>
-          <xdr:rowOff>10252</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2109" name="Object 61" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2109"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E5803F2-B42F-43DF-9A65-985281E9E1AC}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd type="none" w="med" len="med"/>
-            </a:ln>
-            <a:effectLst/>
-            <a:extLst>
-              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                <a14:hiddenEffects>
-                  <a:effectLst>
-                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                      <a:srgbClr val="808080"/>
-                    </a:outerShdw>
-                  </a:effectLst>
-                </a14:hiddenEffects>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
-          <xdr:row>61</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>480060</xdr:colOff>
-          <xdr:row>62</xdr:row>
-          <xdr:rowOff>25044</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2119" name="Object 71" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2119"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2B4D5B9-A7FF-432F-BE05-5F9F9F68B1BA}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd type="none" w="med" len="med"/>
-            </a:ln>
-            <a:effectLst/>
-            <a:extLst>
-              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                <a14:hiddenEffects>
-                  <a:effectLst>
-                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                      <a:srgbClr val="808080"/>
-                    </a:outerShdw>
-                  </a:effectLst>
-                </a14:hiddenEffects>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
-          <xdr:row>60</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>487680</xdr:colOff>
-          <xdr:row>60</xdr:row>
-          <xdr:rowOff>176395</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2120" name="Object 72" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2120"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B97554D4-3EA0-45CD-9C17-5E198507A09C}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd type="none" w="med" len="med"/>
-            </a:ln>
-            <a:effectLst/>
-            <a:extLst>
-              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                <a14:hiddenEffects>
-                  <a:effectLst>
-                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                      <a:srgbClr val="808080"/>
-                    </a:outerShdw>
-                  </a:effectLst>
-                </a14:hiddenEffects>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
-          <xdr:row>59</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>5</xdr:col>
-          <xdr:colOff>195767</xdr:colOff>
-          <xdr:row>60</xdr:row>
-          <xdr:rowOff>7620</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2121" name="Object 73" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2121"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEE3BE6C-4987-42E0-A9BC-CCC6011C9C49}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd type="none" w="med" len="med"/>
-            </a:ln>
-            <a:effectLst/>
-            <a:extLst>
-              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                <a14:hiddenEffects>
-                  <a:effectLst>
-                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                      <a:srgbClr val="808080"/>
-                    </a:outerShdw>
-                  </a:effectLst>
-                </a14:hiddenEffects>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
-          <xdr:row>58</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>533400</xdr:colOff>
-          <xdr:row>58</xdr:row>
-          <xdr:rowOff>171901</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2122" name="Object 74" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2122"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{18AEF411-DDCB-458C-9021-B24C0E5168D2}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-            </a:solidFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd type="none" w="med" len="med"/>
-            </a:ln>
-            <a:effectLst/>
-            <a:extLst>
-              <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-                <a14:hiddenEffects>
-                  <a:effectLst>
-                    <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                      <a:srgbClr val="808080"/>
-                    </a:outerShdw>
-                  </a:effectLst>
-                </a14:hiddenEffects>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>0</xdr:colOff>
-          <xdr:row>57</xdr:row>
-          <xdr:rowOff>0</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>4</xdr:col>
-          <xdr:colOff>541020</xdr:colOff>
-          <xdr:row>57</xdr:row>
-          <xdr:rowOff>179460</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2123" name="Object 75" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s2123"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5DB0256-575F-4ED9-9F95-2C40EEF51456}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC4A1A96-BA53-47E6-A34D-9C5E70BE1085}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3676,8 +4064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S517"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C46" workbookViewId="0">
-      <selection activeCell="I58" sqref="I58"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="F77" sqref="F77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5820,15 +6208,21 @@
       <c r="A63" s="1">
         <v>62</v>
       </c>
-      <c r="B63" s="1"/>
+      <c r="B63" s="3" t="s">
+        <v>153</v>
+      </c>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
-      <c r="G63" s="1"/>
+      <c r="G63" s="1" t="s">
+        <v>125</v>
+      </c>
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
-      <c r="J63" s="1"/>
+      <c r="J63" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="K63" s="1"/>
       <c r="L63" s="1"/>
       <c r="M63" s="1"/>
@@ -5843,15 +6237,21 @@
       <c r="A64" s="1">
         <v>63</v>
       </c>
-      <c r="B64" s="1"/>
+      <c r="B64" s="3" t="s">
+        <v>154</v>
+      </c>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
-      <c r="G64" s="1"/>
+      <c r="G64" s="1" t="s">
+        <v>125</v>
+      </c>
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
-      <c r="J64" s="1"/>
+      <c r="J64" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="K64" s="1"/>
       <c r="L64" s="1"/>
       <c r="M64" s="1"/>
@@ -5866,15 +6266,23 @@
       <c r="A65" s="1">
         <v>64</v>
       </c>
-      <c r="B65" s="1"/>
+      <c r="B65" s="3" t="s">
+        <v>155</v>
+      </c>
       <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
+      <c r="D65" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
-      <c r="G65" s="1"/>
+      <c r="G65" s="1" t="s">
+        <v>125</v>
+      </c>
       <c r="H65" s="1"/>
       <c r="I65" s="1"/>
-      <c r="J65" s="1"/>
+      <c r="J65" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="K65" s="1"/>
       <c r="L65" s="1"/>
       <c r="M65" s="1"/>
@@ -5889,15 +6297,23 @@
       <c r="A66" s="1">
         <v>65</v>
       </c>
-      <c r="B66" s="1"/>
+      <c r="B66" s="3" t="s">
+        <v>156</v>
+      </c>
       <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
+      <c r="D66" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
-      <c r="G66" s="1"/>
+      <c r="G66" s="1" t="s">
+        <v>125</v>
+      </c>
       <c r="H66" s="1"/>
       <c r="I66" s="1"/>
-      <c r="J66" s="1"/>
+      <c r="J66" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="K66" s="1"/>
       <c r="L66" s="1"/>
       <c r="M66" s="1"/>
@@ -5908,42 +6324,52 @@
       <c r="R66" s="1"/>
       <c r="S66" s="1"/>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A67" s="1">
+    <row r="67" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="6">
         <v>66</v>
       </c>
-      <c r="B67" s="1"/>
-      <c r="C67" s="1"/>
-      <c r="D67" s="1"/>
-      <c r="E67" s="1"/>
-      <c r="F67" s="1"/>
-      <c r="G67" s="1"/>
-      <c r="H67" s="1"/>
-      <c r="I67" s="1"/>
-      <c r="J67" s="1"/>
-      <c r="K67" s="1"/>
-      <c r="L67" s="1"/>
-      <c r="M67" s="1"/>
-      <c r="N67" s="1"/>
-      <c r="O67" s="1"/>
-      <c r="P67" s="1"/>
-      <c r="Q67" s="1"/>
-      <c r="R67" s="1"/>
-      <c r="S67" s="1"/>
+      <c r="B67" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="C67" s="6"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="6"/>
+      <c r="G67" s="6"/>
+      <c r="H67" s="6"/>
+      <c r="I67" s="6"/>
+      <c r="J67" s="6"/>
+      <c r="K67" s="6"/>
+      <c r="L67" s="6"/>
+      <c r="M67" s="6"/>
+      <c r="N67" s="6"/>
+      <c r="O67" s="6"/>
+      <c r="P67" s="6"/>
+      <c r="Q67" s="6"/>
+      <c r="R67" s="6"/>
+      <c r="S67" s="6"/>
     </row>
     <row r="68" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>67</v>
       </c>
-      <c r="B68" s="1"/>
+      <c r="B68" s="3" t="s">
+        <v>158</v>
+      </c>
       <c r="C68" s="1"/>
-      <c r="D68" s="1"/>
+      <c r="D68" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
-      <c r="G68" s="1"/>
+      <c r="G68" s="1" t="s">
+        <v>157</v>
+      </c>
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
-      <c r="J68" s="1"/>
+      <c r="J68" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="K68" s="1"/>
       <c r="L68" s="1"/>
       <c r="M68" s="1"/>
@@ -5958,15 +6384,23 @@
       <c r="A69" s="1">
         <v>68</v>
       </c>
-      <c r="B69" s="1"/>
+      <c r="B69" s="3" t="s">
+        <v>159</v>
+      </c>
       <c r="C69" s="1"/>
-      <c r="D69" s="1"/>
+      <c r="D69" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
-      <c r="G69" s="1"/>
+      <c r="G69" s="1" t="s">
+        <v>157</v>
+      </c>
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
-      <c r="J69" s="1"/>
+      <c r="J69" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="K69" s="1"/>
       <c r="L69" s="1"/>
       <c r="M69" s="1"/>
@@ -5981,15 +6415,23 @@
       <c r="A70" s="1">
         <v>69</v>
       </c>
-      <c r="B70" s="1"/>
+      <c r="B70" s="3" t="s">
+        <v>162</v>
+      </c>
       <c r="C70" s="1"/>
-      <c r="D70" s="1"/>
+      <c r="D70" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
-      <c r="G70" s="1"/>
+      <c r="G70" s="1" t="s">
+        <v>157</v>
+      </c>
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
-      <c r="J70" s="1"/>
+      <c r="J70" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="K70" s="1"/>
       <c r="L70" s="1"/>
       <c r="M70" s="1"/>
@@ -6004,15 +6446,23 @@
       <c r="A71" s="1">
         <v>70</v>
       </c>
-      <c r="B71" s="1"/>
+      <c r="B71" s="1" t="s">
+        <v>157</v>
+      </c>
       <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
+      <c r="D71" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
-      <c r="G71" s="1"/>
+      <c r="G71" s="1" t="s">
+        <v>157</v>
+      </c>
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
-      <c r="J71" s="1"/>
+      <c r="J71" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="K71" s="1"/>
       <c r="L71" s="1"/>
       <c r="M71" s="1"/>
@@ -6027,15 +6477,23 @@
       <c r="A72" s="1">
         <v>71</v>
       </c>
-      <c r="B72" s="1"/>
+      <c r="B72" s="1" t="s">
+        <v>161</v>
+      </c>
       <c r="C72" s="1"/>
-      <c r="D72" s="1"/>
+      <c r="D72" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
-      <c r="G72" s="1"/>
+      <c r="G72" s="1" t="s">
+        <v>157</v>
+      </c>
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
-      <c r="J72" s="1"/>
+      <c r="J72" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="K72" s="1"/>
       <c r="L72" s="1"/>
       <c r="M72" s="1"/>
@@ -6050,15 +6508,23 @@
       <c r="A73" s="1">
         <v>72</v>
       </c>
-      <c r="B73" s="1"/>
+      <c r="B73" s="1" t="s">
+        <v>160</v>
+      </c>
       <c r="C73" s="1"/>
-      <c r="D73" s="1"/>
+      <c r="D73" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
-      <c r="G73" s="1"/>
+      <c r="G73" s="1" t="s">
+        <v>157</v>
+      </c>
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
-      <c r="J73" s="1"/>
+      <c r="J73" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="K73" s="1"/>
       <c r="L73" s="1"/>
       <c r="M73" s="1"/>
@@ -6073,15 +6539,23 @@
       <c r="A74" s="1">
         <v>73</v>
       </c>
-      <c r="B74" s="1"/>
+      <c r="B74" s="1" t="s">
+        <v>163</v>
+      </c>
       <c r="C74" s="1"/>
-      <c r="D74" s="1"/>
+      <c r="D74" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
-      <c r="G74" s="1"/>
+      <c r="G74" s="1" t="s">
+        <v>157</v>
+      </c>
       <c r="H74" s="1"/>
       <c r="I74" s="1"/>
-      <c r="J74" s="1"/>
+      <c r="J74" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="K74" s="1"/>
       <c r="L74" s="1"/>
       <c r="M74" s="1"/>
@@ -6096,15 +6570,23 @@
       <c r="A75" s="1">
         <v>74</v>
       </c>
-      <c r="B75" s="1"/>
+      <c r="B75" s="3" t="s">
+        <v>164</v>
+      </c>
       <c r="C75" s="1"/>
-      <c r="D75" s="1"/>
+      <c r="D75" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
-      <c r="G75" s="1"/>
+      <c r="G75" s="1" t="s">
+        <v>157</v>
+      </c>
       <c r="H75" s="1"/>
       <c r="I75" s="1"/>
-      <c r="J75" s="1"/>
+      <c r="J75" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="K75" s="1"/>
       <c r="L75" s="1"/>
       <c r="M75" s="1"/>
@@ -6119,15 +6601,23 @@
       <c r="A76" s="1">
         <v>75</v>
       </c>
-      <c r="B76" s="1"/>
+      <c r="B76" s="3" t="s">
+        <v>165</v>
+      </c>
       <c r="C76" s="1"/>
-      <c r="D76" s="1"/>
+      <c r="D76" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
-      <c r="G76" s="1"/>
+      <c r="G76" s="1" t="s">
+        <v>157</v>
+      </c>
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
-      <c r="J76" s="1"/>
+      <c r="J76" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="K76" s="1"/>
       <c r="L76" s="1"/>
       <c r="M76" s="1"/>
@@ -6150,7 +6640,9 @@
       <c r="G77" s="1"/>
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
-      <c r="J77" s="1"/>
+      <c r="J77" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="K77" s="1"/>
       <c r="L77" s="1"/>
       <c r="M77" s="1"/>
@@ -16284,7 +16776,7 @@
   </sheetData>
   <autoFilter ref="A1:S1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1:J1048576" xr:uid="{9D6440E9-8E1E-43AC-B858-E4572FF2CA51}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1:J66 J68:J1048576" xr:uid="{9D6440E9-8E1E-43AC-B858-E4572FF2CA51}">
       <formula1>"Scaler-A,Scaler-I,Leetcode,GFG"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D1048576" xr:uid="{BF20C4B6-E8A1-4D23-A148-D05D51CB2238}">
@@ -16336,16 +16828,25 @@
     <hyperlink ref="B61" r:id="rId42" xr:uid="{2A7B61F4-5927-4932-91B6-8E2D2141BB0A}"/>
     <hyperlink ref="B60" r:id="rId43" xr:uid="{EFDD7B76-A14F-44C6-8D18-C1AD631593DA}"/>
     <hyperlink ref="B57" r:id="rId44" xr:uid="{D9A93759-E682-4FB4-B1CB-AE372A2360D1}"/>
+    <hyperlink ref="B66" r:id="rId45" xr:uid="{4FA4C7EE-27DD-4DDB-AD83-51320B3A1C00}"/>
+    <hyperlink ref="B65" r:id="rId46" xr:uid="{02DB27FC-F420-4533-8761-2E5EC3E01E5B}"/>
+    <hyperlink ref="B64" r:id="rId47" xr:uid="{553B31AF-1E9F-44F9-A5A7-29531D33DC23}"/>
+    <hyperlink ref="B63" r:id="rId48" xr:uid="{F549B0B0-A722-476E-97AE-BE49AAFE9CAB}"/>
+    <hyperlink ref="B68" r:id="rId49" xr:uid="{86DD804E-9B05-47CF-8105-1FA442E4DE70}"/>
+    <hyperlink ref="B69" r:id="rId50" xr:uid="{B1AB2FBA-B312-4B4C-9BA3-9CC5EEE28C28}"/>
+    <hyperlink ref="B70" r:id="rId51" xr:uid="{94F0704A-9350-4C36-92B9-E5BD93A5EBA2}"/>
+    <hyperlink ref="B75" r:id="rId52" xr:uid="{852A4C53-9195-4428-ABAF-5D0A73E99ECF}"/>
+    <hyperlink ref="B76" r:id="rId53" xr:uid="{388BD0C9-2ADE-4ED6-A33A-6A603C9A678F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId45"/>
-  <drawing r:id="rId46"/>
-  <legacyDrawing r:id="rId47"/>
+  <pageSetup orientation="portrait" r:id="rId54"/>
+  <drawing r:id="rId55"/>
+  <legacyDrawing r:id="rId56"/>
   <oleObjects>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="2049" r:id="rId48">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId49">
+        <oleObject progId="Packager Shell Object" shapeId="2049" r:id="rId57">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId58">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -16364,13 +16865,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="2049" r:id="rId48"/>
+        <oleObject progId="Packager Shell Object" shapeId="2049" r:id="rId57"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="2052" r:id="rId50">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId51">
+        <oleObject progId="Packager Shell Object" shapeId="2052" r:id="rId59">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId60">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -16389,13 +16890,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="2052" r:id="rId50"/>
+        <oleObject progId="Packager Shell Object" shapeId="2052" r:id="rId59"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="2053" r:id="rId52">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId53">
+        <oleObject progId="Packager Shell Object" shapeId="2053" r:id="rId61">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId62">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -16414,13 +16915,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="2053" r:id="rId52"/>
+        <oleObject progId="Packager Shell Object" shapeId="2053" r:id="rId61"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="2054" r:id="rId54">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId55">
+        <oleObject progId="Packager Shell Object" shapeId="2054" r:id="rId63">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId64">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -16439,13 +16940,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="2054" r:id="rId54"/>
+        <oleObject progId="Packager Shell Object" shapeId="2054" r:id="rId63"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="2055" r:id="rId56">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId57">
+        <oleObject progId="Packager Shell Object" shapeId="2055" r:id="rId65">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId66">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -16464,13 +16965,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="2055" r:id="rId56"/>
+        <oleObject progId="Packager Shell Object" shapeId="2055" r:id="rId65"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="2056" r:id="rId58">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId59">
+        <oleObject progId="Packager Shell Object" shapeId="2056" r:id="rId67">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId68">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -16489,13 +16990,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="2056" r:id="rId58"/>
+        <oleObject progId="Packager Shell Object" shapeId="2056" r:id="rId67"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="2057" r:id="rId60">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId61">
+        <oleObject progId="Packager Shell Object" shapeId="2057" r:id="rId69">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId70">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -16514,13 +17015,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="2057" r:id="rId60"/>
+        <oleObject progId="Packager Shell Object" shapeId="2057" r:id="rId69"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="2058" r:id="rId62">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId63">
+        <oleObject progId="Packager Shell Object" shapeId="2058" r:id="rId71">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId72">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -16539,13 +17040,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="2058" r:id="rId62"/>
+        <oleObject progId="Packager Shell Object" shapeId="2058" r:id="rId71"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="2059" r:id="rId64">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId65">
+        <oleObject progId="Packager Shell Object" shapeId="2059" r:id="rId73">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId74">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -16564,13 +17065,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="2059" r:id="rId64"/>
+        <oleObject progId="Packager Shell Object" shapeId="2059" r:id="rId73"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="2060" r:id="rId66">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId67">
+        <oleObject progId="Packager Shell Object" shapeId="2060" r:id="rId75">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId76">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -16589,13 +17090,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="2060" r:id="rId66"/>
+        <oleObject progId="Packager Shell Object" shapeId="2060" r:id="rId75"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="2061" r:id="rId68">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId69">
+        <oleObject progId="Packager Shell Object" shapeId="2061" r:id="rId77">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId78">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -16614,13 +17115,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="2061" r:id="rId68"/>
+        <oleObject progId="Packager Shell Object" shapeId="2061" r:id="rId77"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="2062" r:id="rId70">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId71">
+        <oleObject progId="Packager Shell Object" shapeId="2062" r:id="rId79">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId80">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -16639,13 +17140,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="2062" r:id="rId70"/>
+        <oleObject progId="Packager Shell Object" shapeId="2062" r:id="rId79"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="2063" r:id="rId72">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId73">
+        <oleObject progId="Packager Shell Object" shapeId="2063" r:id="rId81">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId82">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -16664,13 +17165,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="2063" r:id="rId72"/>
+        <oleObject progId="Packager Shell Object" shapeId="2063" r:id="rId81"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="2064" r:id="rId74">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId75">
+        <oleObject progId="Packager Shell Object" shapeId="2064" r:id="rId83">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId84">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -16689,13 +17190,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="2064" r:id="rId74"/>
+        <oleObject progId="Packager Shell Object" shapeId="2064" r:id="rId83"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="2065" r:id="rId76">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId77">
+        <oleObject progId="Packager Shell Object" shapeId="2065" r:id="rId85">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId86">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -16714,13 +17215,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="2065" r:id="rId76"/>
+        <oleObject progId="Packager Shell Object" shapeId="2065" r:id="rId85"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="2066" r:id="rId78">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId79">
+        <oleObject progId="Packager Shell Object" shapeId="2066" r:id="rId87">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId88">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -16739,13 +17240,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="2066" r:id="rId78"/>
+        <oleObject progId="Packager Shell Object" shapeId="2066" r:id="rId87"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="2067" r:id="rId80">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId81">
+        <oleObject progId="Packager Shell Object" shapeId="2067" r:id="rId89">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId90">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -16764,13 +17265,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="2067" r:id="rId80"/>
+        <oleObject progId="Packager Shell Object" shapeId="2067" r:id="rId89"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="2068" r:id="rId82">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId83">
+        <oleObject progId="Packager Shell Object" shapeId="2068" r:id="rId91">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId92">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -16789,13 +17290,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="2068" r:id="rId82"/>
+        <oleObject progId="Packager Shell Object" shapeId="2068" r:id="rId91"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="2072" r:id="rId84">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId85">
+        <oleObject progId="Packager Shell Object" shapeId="2072" r:id="rId93">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId94">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -16814,13 +17315,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="2072" r:id="rId84"/>
+        <oleObject progId="Packager Shell Object" shapeId="2072" r:id="rId93"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="2073" r:id="rId86">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId87">
+        <oleObject progId="Packager Shell Object" shapeId="2073" r:id="rId95">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId96">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -16839,13 +17340,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="2073" r:id="rId86"/>
+        <oleObject progId="Packager Shell Object" shapeId="2073" r:id="rId95"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="2076" r:id="rId88">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId89">
+        <oleObject progId="Packager Shell Object" shapeId="2076" r:id="rId97">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId98">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -16864,13 +17365,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="2076" r:id="rId88"/>
+        <oleObject progId="Packager Shell Object" shapeId="2076" r:id="rId97"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="2082" r:id="rId90">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId91">
+        <oleObject progId="Packager Shell Object" shapeId="2082" r:id="rId99">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId100">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -16889,13 +17390,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="2082" r:id="rId90"/>
+        <oleObject progId="Packager Shell Object" shapeId="2082" r:id="rId99"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="2083" r:id="rId92">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId93">
+        <oleObject progId="Packager Shell Object" shapeId="2083" r:id="rId101">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId102">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -16914,13 +17415,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="2083" r:id="rId92"/>
+        <oleObject progId="Packager Shell Object" shapeId="2083" r:id="rId101"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="2084" r:id="rId94">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId95">
+        <oleObject progId="Packager Shell Object" shapeId="2084" r:id="rId103">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId104">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -16939,13 +17440,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="2084" r:id="rId94"/>
+        <oleObject progId="Packager Shell Object" shapeId="2084" r:id="rId103"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="2086" r:id="rId96">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId97">
+        <oleObject progId="Packager Shell Object" shapeId="2086" r:id="rId105">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId106">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -16964,13 +17465,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="2086" r:id="rId96"/>
+        <oleObject progId="Packager Shell Object" shapeId="2086" r:id="rId105"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="2087" r:id="rId98">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId99">
+        <oleObject progId="Packager Shell Object" shapeId="2087" r:id="rId107">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId108">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -16989,13 +17490,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="2087" r:id="rId98"/>
+        <oleObject progId="Packager Shell Object" shapeId="2087" r:id="rId107"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="2088" r:id="rId100">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId101">
+        <oleObject progId="Packager Shell Object" shapeId="2088" r:id="rId109">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId110">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -17014,13 +17515,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="2088" r:id="rId100"/>
+        <oleObject progId="Packager Shell Object" shapeId="2088" r:id="rId109"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="2091" r:id="rId102">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId103">
+        <oleObject progId="Packager Shell Object" shapeId="2091" r:id="rId111">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId112">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -17039,13 +17540,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="2091" r:id="rId102"/>
+        <oleObject progId="Packager Shell Object" shapeId="2091" r:id="rId111"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="2092" r:id="rId104">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId105">
+        <oleObject progId="Packager Shell Object" shapeId="2092" r:id="rId113">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId114">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -17064,13 +17565,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="2092" r:id="rId104"/>
+        <oleObject progId="Packager Shell Object" shapeId="2092" r:id="rId113"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="2093" r:id="rId106">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId107">
+        <oleObject progId="Packager Shell Object" shapeId="2093" r:id="rId115">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId116">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -17089,13 +17590,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="2093" r:id="rId106"/>
+        <oleObject progId="Packager Shell Object" shapeId="2093" r:id="rId115"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="2099" r:id="rId108">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId109">
+        <oleObject progId="Packager Shell Object" shapeId="2099" r:id="rId117">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId118">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -17114,13 +17615,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="2099" r:id="rId108"/>
+        <oleObject progId="Packager Shell Object" shapeId="2099" r:id="rId117"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="2100" r:id="rId110">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId111">
+        <oleObject progId="Packager Shell Object" shapeId="2100" r:id="rId119">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId120">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -17139,13 +17640,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="2100" r:id="rId110"/>
+        <oleObject progId="Packager Shell Object" shapeId="2100" r:id="rId119"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="2101" r:id="rId112">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId113">
+        <oleObject progId="Packager Shell Object" shapeId="2101" r:id="rId121">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId122">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -17164,13 +17665,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="2101" r:id="rId112"/>
+        <oleObject progId="Packager Shell Object" shapeId="2101" r:id="rId121"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="2102" r:id="rId114">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId115">
+        <oleObject progId="Packager Shell Object" shapeId="2102" r:id="rId123">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId124">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -17189,13 +17690,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="2102" r:id="rId114"/>
+        <oleObject progId="Packager Shell Object" shapeId="2102" r:id="rId123"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="2104" r:id="rId116">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId117">
+        <oleObject progId="Packager Shell Object" shapeId="2104" r:id="rId125">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId126">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -17214,13 +17715,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="2104" r:id="rId116"/>
+        <oleObject progId="Packager Shell Object" shapeId="2104" r:id="rId125"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="2105" r:id="rId118">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId119">
+        <oleObject progId="Packager Shell Object" shapeId="2105" r:id="rId127">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId128">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -17239,13 +17740,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="2105" r:id="rId118"/>
+        <oleObject progId="Packager Shell Object" shapeId="2105" r:id="rId127"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="2106" r:id="rId120">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId121">
+        <oleObject progId="Packager Shell Object" shapeId="2106" r:id="rId129">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId130">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -17264,13 +17765,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="2106" r:id="rId120"/>
+        <oleObject progId="Packager Shell Object" shapeId="2106" r:id="rId129"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="2107" r:id="rId122">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId123">
+        <oleObject progId="Packager Shell Object" shapeId="2107" r:id="rId131">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId132">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -17289,13 +17790,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="2107" r:id="rId122"/>
+        <oleObject progId="Packager Shell Object" shapeId="2107" r:id="rId131"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="2108" r:id="rId124">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId125">
+        <oleObject progId="Packager Shell Object" shapeId="2108" r:id="rId133">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId134">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -17314,13 +17815,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="2108" r:id="rId124"/>
+        <oleObject progId="Packager Shell Object" shapeId="2108" r:id="rId133"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="2109" r:id="rId126">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId127">
+        <oleObject progId="Packager Shell Object" shapeId="2109" r:id="rId135">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId136">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -17339,13 +17840,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="2109" r:id="rId126"/>
+        <oleObject progId="Packager Shell Object" shapeId="2109" r:id="rId135"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="2119" r:id="rId128">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId129">
+        <oleObject progId="Packager Shell Object" shapeId="2119" r:id="rId137">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId138">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -17364,13 +17865,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="2119" r:id="rId128"/>
+        <oleObject progId="Packager Shell Object" shapeId="2119" r:id="rId137"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="2120" r:id="rId130">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId131">
+        <oleObject progId="Packager Shell Object" shapeId="2120" r:id="rId139">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId140">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -17389,13 +17890,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="2120" r:id="rId130"/>
+        <oleObject progId="Packager Shell Object" shapeId="2120" r:id="rId139"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="2121" r:id="rId132">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId133">
+        <oleObject progId="Packager Shell Object" shapeId="2121" r:id="rId141">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId142">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -17414,13 +17915,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="2121" r:id="rId132"/>
+        <oleObject progId="Packager Shell Object" shapeId="2121" r:id="rId141"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="2122" r:id="rId134">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId135">
+        <oleObject progId="Packager Shell Object" shapeId="2122" r:id="rId143">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId144">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -17439,13 +17940,13 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="2122" r:id="rId134"/>
+        <oleObject progId="Packager Shell Object" shapeId="2122" r:id="rId143"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <oleObject progId="Packager Shell Object" shapeId="2123" r:id="rId136">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId137">
+        <oleObject progId="Packager Shell Object" shapeId="2123" r:id="rId145">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId146">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>4</xdr:col>
@@ -17464,7 +17965,207 @@
         </oleObject>
       </mc:Choice>
       <mc:Fallback>
-        <oleObject progId="Packager Shell Object" shapeId="2123" r:id="rId136"/>
+        <oleObject progId="Packager Shell Object" shapeId="2123" r:id="rId145"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Packager Shell Object" shapeId="2128" r:id="rId147">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId148">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>67</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>502920</xdr:colOff>
+                <xdr:row>67</xdr:row>
+                <xdr:rowOff>167640</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Packager Shell Object" shapeId="2128" r:id="rId147"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Packager Shell Object" shapeId="2129" r:id="rId149">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId150">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>68</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>175260</xdr:colOff>
+                <xdr:row>68</xdr:row>
+                <xdr:rowOff>175260</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Packager Shell Object" shapeId="2129" r:id="rId149"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Packager Shell Object" shapeId="2130" r:id="rId151">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId152">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>69</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>365760</xdr:colOff>
+                <xdr:row>69</xdr:row>
+                <xdr:rowOff>167640</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Packager Shell Object" shapeId="2130" r:id="rId151"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Packager Shell Object" shapeId="2131" r:id="rId153">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId154">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>70</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>388620</xdr:colOff>
+                <xdr:row>70</xdr:row>
+                <xdr:rowOff>182880</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Packager Shell Object" shapeId="2131" r:id="rId153"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Packager Shell Object" shapeId="2132" r:id="rId155">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId156">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>71</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>411480</xdr:colOff>
+                <xdr:row>72</xdr:row>
+                <xdr:rowOff>7620</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Packager Shell Object" shapeId="2132" r:id="rId155"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Packager Shell Object" shapeId="2133" r:id="rId157">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId158">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>72</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>449580</xdr:colOff>
+                <xdr:row>73</xdr:row>
+                <xdr:rowOff>15240</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Packager Shell Object" shapeId="2133" r:id="rId157"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Packager Shell Object" shapeId="2134" r:id="rId159">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId160">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>73</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>403860</xdr:colOff>
+                <xdr:row>74</xdr:row>
+                <xdr:rowOff>7620</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Packager Shell Object" shapeId="2134" r:id="rId159"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Packager Shell Object" shapeId="2135" r:id="rId161">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId162">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>74</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>701040</xdr:colOff>
+                <xdr:row>75</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Packager Shell Object" shapeId="2135" r:id="rId161"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </oleObjects>

</xml_diff>